<commit_message>
Home page label for negative scenario
</commit_message>
<xml_diff>
--- a/Task1Test/src/main/java/com/app/qa/testdata/TestDataForAutomation.xlsx
+++ b/Task1Test/src/main/java/com/app/qa/testdata/TestDataForAutomation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suman\eclipse-workspace\POM\Task1Test\src\main\java\com\app\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suman\git\TestAutomationFramework\Task1Test\src\main\java\com\app\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A07533-25A6-462D-876B-B91B6A88FCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65ABC1B7-DCC4-4DB2-84A7-CEC58F104E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Title</t>
   </si>
@@ -42,18 +42,9 @@
     <t>Mr.</t>
   </si>
   <si>
-    <t>Harley</t>
-  </si>
-  <si>
-    <t>Dion</t>
-  </si>
-  <si>
     <t>Persistent</t>
   </si>
   <si>
-    <t>Xinjon</t>
-  </si>
-  <si>
     <t>Su</t>
   </si>
   <si>
@@ -70,6 +61,36 @@
   </si>
   <si>
     <t>Prof.</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Watt</t>
+  </si>
+  <si>
+    <t>Bazun</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>Zia</t>
+  </si>
+  <si>
+    <t>Gill</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Sir</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>Paul</t>
   </si>
 </sst>
 </file>
@@ -402,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,41 +454,69 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>